<commit_message>
update gh since last flurry
</commit_message>
<xml_diff>
--- a/FLAGS.xlsx
+++ b/FLAGS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/blairmunroakusa/_ROOT/___LEAF/fracpay/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{267A3072-EA62-3F4E-BFB4-7A0D1D179896}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4AB6D2-3B43-F848-8A34-E8DE3294C2A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="500" windowWidth="18880" windowHeight="23500" xr2:uid="{910C8346-B54A-654B-BBFB-9AB65F69FD92}"/>
+    <workbookView minimized="1" xWindow="660" yWindow="500" windowWidth="18880" windowHeight="23500" xr2:uid="{910C8346-B54A-654B-BBFB-9AB65F69FD92}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="45">
   <si>
     <t>x</t>
   </si>
@@ -48,9 +48,6 @@
     <t>R</t>
   </si>
   <si>
-    <t>P</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
@@ -160,6 +157,18 @@
   </si>
   <si>
     <t>INVITATION?</t>
+  </si>
+  <si>
+    <t>BUSY</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -645,7 +654,7 @@
   <dimension ref="A4:V21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S21" sqref="S21"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -655,36 +664,36 @@
   <sheetData>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="8"/>
       <c r="D4" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E4" s="8"/>
       <c r="H4" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
       <c r="U4" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="V4" s="8"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
@@ -694,21 +703,21 @@
         <v>0</v>
       </c>
       <c r="V5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K6" s="8"/>
       <c r="L6" s="8"/>
@@ -718,22 +727,22 @@
         <v>1</v>
       </c>
       <c r="V6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
@@ -742,10 +751,10 @@
     </row>
     <row r="8" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" s="4"/>
       <c r="H8" s="3"/>
@@ -753,16 +762,16 @@
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="U8" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="V8" s="8"/>
     </row>
     <row r="9" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>1</v>
@@ -777,22 +786,22 @@
         <v>1</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K9" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="L9" s="2" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="N9" s="2" t="s">
         <v>0</v>
@@ -816,15 +825,15 @@
         <v>0</v>
       </c>
       <c r="V9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -853,108 +862,117 @@
       <c r="L10" s="11">
         <v>8</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="11">
         <v>9</v>
       </c>
       <c r="U10">
         <v>1</v>
       </c>
       <c r="V10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
       <c r="U12" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="V12" s="8"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
       <c r="U13">
         <v>0</v>
       </c>
       <c r="V13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
       <c r="U14">
         <v>1</v>
       </c>
       <c r="V14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L15" s="3"/>
+      <c r="M15" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M16" s="8"/>
       <c r="N16" s="8"/>
       <c r="O16" s="8"/>
       <c r="P16" s="8"/>
       <c r="U16" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="V16" s="8"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
         <v>27</v>
-      </c>
-      <c r="B17" t="s">
-        <v>28</v>
       </c>
       <c r="U17">
         <v>0</v>
       </c>
       <c r="V17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.2">
@@ -962,13 +980,13 @@
         <v>1101</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="U18">
         <v>1</v>
       </c>
       <c r="V18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.2">
@@ -976,7 +994,7 @@
         <v>1110</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.2">
@@ -984,7 +1002,7 @@
         <v>1111</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.2">

</xml_diff>